<commit_message>
FT ERM2022 - v05 actualizado
</commit_message>
<xml_diff>
--- a/CONTROL Y MODIFICACION SISGLV ERM 2022(4).xlsx
+++ b/CONTROL Y MODIFICACION SISGLV ERM 2022(4).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ONPE\DOCUMENTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ONPE\Repositorio ONPE\repositorioOnpe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="0" windowWidth="22104" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="3744" yWindow="0" windowWidth="22104" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SISGLV" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
   <si>
     <t>ID_LOCAL</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>SE MOVIERON AMBIENTES ESPECIALES; SE MOVIERON AULAS DEL PABELLON</t>
+  </si>
+  <si>
+    <t>SE MOVIERON AMBIENTES ESPECIALES; SE AGREGO UN AULA DEL PABELLON 200 Y 300; SE MOVIERON AULAS DEL PABELLONE 100</t>
   </si>
 </sst>
 </file>
@@ -401,13 +404,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,12 +846,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1385,7 +1388,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,12 +1401,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" s="10" customFormat="1" ht="10.8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1566,7 +1569,7 @@
       <c r="B13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -1580,7 +1583,7 @@
       <c r="B14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -1594,7 +1597,7 @@
       <c r="B15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -1608,7 +1611,7 @@
       <c r="B16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -1622,7 +1625,7 @@
       <c r="B17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -1636,7 +1639,7 @@
       <c r="B18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="12" t="s">
@@ -1650,7 +1653,7 @@
       <c r="B19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="12" t="s">
@@ -1664,7 +1667,7 @@
       <c r="B20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="12" t="s">
@@ -1678,7 +1681,7 @@
       <c r="B21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -1692,7 +1695,7 @@
       <c r="B22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -1706,7 +1709,7 @@
       <c r="B23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -1720,7 +1723,7 @@
       <c r="B24" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -1734,7 +1737,7 @@
       <c r="B25" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -1748,7 +1751,7 @@
       <c r="B26" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -1762,7 +1765,7 @@
       <c r="B27" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="12" t="s">
@@ -1776,7 +1779,7 @@
       <c r="B28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="14" t="s">
         <v>45</v>
       </c>
       <c r="D28" s="12" t="s">
@@ -1790,7 +1793,7 @@
       <c r="B29" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D29" s="12" t="s">
@@ -1804,7 +1807,7 @@
       <c r="B30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D30" s="12" t="s">
@@ -1818,7 +1821,7 @@
       <c r="B31" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D31" s="12" t="s">
@@ -1832,7 +1835,7 @@
       <c r="B32" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="14" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="12" t="s">
@@ -1846,7 +1849,7 @@
       <c r="B33" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D33" s="12" t="s">
@@ -1860,7 +1863,7 @@
       <c r="B34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="14" t="s">
         <v>55</v>
       </c>
       <c r="D34" s="12" t="s">
@@ -1874,7 +1877,7 @@
       <c r="B35" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="14">
         <v>4909</v>
       </c>
       <c r="D35" s="12" t="s">
@@ -1888,7 +1891,7 @@
       <c r="B36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D36" s="12" t="s">
@@ -1920,7 +1923,7 @@
         <v>4936</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>